<commit_message>
pushing wash, education & protection indicators
</commit_message>
<xml_diff>
--- a/input/indicators/Protection list of indicators 2021_final.xlsx
+++ b/input/indicators/Protection list of indicators 2021_final.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOM-LAP-198\OneDrive - ACTED\DSA_2021\3_Prioritization matrix\LSG scoring\Protection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed Mahamoud\OneDrive - ACTED\1.REACH_Somalia\3.DSA\DSA_V\05_Analysis\SOM2103_DSA_21\input\indicators\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey 2021" sheetId="1" r:id="rId1"/>
@@ -4048,14 +4048,20 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4077,12 +4083,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4416,22 +4416,22 @@
       <selection pane="bottomLeft" activeCell="B342" sqref="B342"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.453125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="46.453125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="45.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="29.36328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="47.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.54296875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" style="1" customWidth="1"/>
-    <col min="10" max="28" width="21.36328125" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="24.453125" style="1"/>
+    <col min="1" max="1" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="46.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="45.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="47.21875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="1" customWidth="1"/>
+    <col min="10" max="28" width="21.33203125" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="24.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>1129</v>
       </c>
@@ -4520,7 +4520,7 @@
       <c r="AD1" s="26"/>
       <c r="AE1" s="26"/>
     </row>
-    <row r="2" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" s="24" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" s="24" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24">
         <v>5</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:31" s="24" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" s="24" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
         <v>6</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4694,7 +4694,7 @@
       <c r="AA9" s="11"/>
       <c r="AB9" s="11"/>
     </row>
-    <row r="10" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4723,7 +4723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4823,7 +4823,7 @@
       <c r="AA13" s="21"/>
       <c r="AB13" s="21"/>
     </row>
-    <row r="14" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4865,7 +4865,7 @@
       <c r="AA14" s="21"/>
       <c r="AB14" s="21"/>
     </row>
-    <row r="15" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4907,7 +4907,7 @@
       <c r="AA15" s="21"/>
       <c r="AB15" s="21"/>
     </row>
-    <row r="16" spans="1:31" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4943,7 +4943,7 @@
       <c r="AA16" s="7"/>
       <c r="AB16" s="7"/>
     </row>
-    <row r="17" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -5016,7 +5016,7 @@
       </c>
       <c r="P19" s="21"/>
     </row>
-    <row r="20" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -5030,7 +5030,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -5054,7 +5054,7 @@
       </c>
       <c r="P21" s="21"/>
     </row>
-    <row r="22" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5083,7 +5083,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -5121,7 +5121,7 @@
       <c r="AA23" s="5"/>
       <c r="AB23" s="5"/>
     </row>
-    <row r="24" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5159,7 +5159,7 @@
       <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
     </row>
-    <row r="25" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5218,7 +5218,7 @@
       <c r="AA26" s="11"/>
       <c r="AB26" s="11"/>
     </row>
-    <row r="27" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5311,7 +5311,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5349,7 +5349,7 @@
       <c r="AA30" s="3"/>
       <c r="AB30" s="3"/>
     </row>
-    <row r="31" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -5391,7 +5391,7 @@
       <c r="AA31" s="11"/>
       <c r="AB31" s="11"/>
     </row>
-    <row r="32" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -5433,7 +5433,7 @@
       <c r="AA32" s="7"/>
       <c r="AB32" s="7"/>
     </row>
-    <row r="33" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -5473,7 +5473,7 @@
       <c r="AA33" s="7"/>
       <c r="AB33" s="7"/>
     </row>
-    <row r="34" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -5511,7 +5511,7 @@
       <c r="AA34" s="7"/>
       <c r="AB34" s="7"/>
     </row>
-    <row r="35" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -5566,7 +5566,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="37" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -5656,7 +5656,7 @@
       <c r="AA39" s="5"/>
       <c r="AB39" s="5"/>
     </row>
-    <row r="40" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -5698,7 +5698,7 @@
       <c r="AA40" s="11"/>
       <c r="AB40" s="11"/>
     </row>
-    <row r="41" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -5818,7 +5818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -5856,7 +5856,7 @@
       <c r="AA47" s="5"/>
       <c r="AB47" s="5"/>
     </row>
-    <row r="48" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -5894,7 +5894,7 @@
       <c r="AA48" s="7"/>
       <c r="AB48" s="7"/>
     </row>
-    <row r="49" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -5963,7 +5963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -5986,7 +5986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -6085,7 +6085,7 @@
       <c r="AA55" s="5"/>
       <c r="AB55" s="5"/>
     </row>
-    <row r="56" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -6123,7 +6123,7 @@
       <c r="AA56" s="7"/>
       <c r="AB56" s="7"/>
     </row>
-    <row r="57" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -6149,7 +6149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -6201,7 +6201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -6239,7 +6239,7 @@
       <c r="AA60" s="5"/>
       <c r="AB60" s="5"/>
     </row>
-    <row r="61" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -6277,7 +6277,7 @@
       <c r="AA61" s="3"/>
       <c r="AB61" s="3"/>
     </row>
-    <row r="62" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -6317,7 +6317,7 @@
       <c r="AA62" s="11"/>
       <c r="AB62" s="11"/>
     </row>
-    <row r="63" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -6355,7 +6355,7 @@
       <c r="AA63" s="7"/>
       <c r="AB63" s="7"/>
     </row>
-    <row r="64" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -6384,7 +6384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -6448,7 +6448,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -6465,7 +6465,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -6525,7 +6525,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -6563,7 +6563,7 @@
       <c r="AA71" s="5"/>
       <c r="AB71" s="5"/>
     </row>
-    <row r="72" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -6580,7 +6580,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -6609,7 +6609,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -6647,7 +6647,7 @@
       <c r="AA74" s="7"/>
       <c r="AB74" s="7"/>
     </row>
-    <row r="75" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -6676,7 +6676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -6699,7 +6699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -6737,7 +6737,7 @@
       <c r="AA77" s="5"/>
       <c r="AB77" s="5"/>
     </row>
-    <row r="78" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -6775,7 +6775,7 @@
       <c r="AA78" s="7"/>
       <c r="AB78" s="7"/>
     </row>
-    <row r="79" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -6798,7 +6798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -6835,7 +6835,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -6873,7 +6873,7 @@
       <c r="AA82" s="5"/>
       <c r="AB82" s="5"/>
     </row>
-    <row r="83" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -6909,7 +6909,7 @@
       <c r="AA83" s="7"/>
       <c r="AB83" s="7"/>
     </row>
-    <row r="84" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="87" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -7017,7 +7017,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="88" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -7040,7 +7040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -7069,7 +7069,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -7124,7 +7124,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -7147,7 +7147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -7208,7 +7208,7 @@
       <c r="AA94" s="5"/>
       <c r="AB94" s="5"/>
     </row>
-    <row r="95" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -7246,7 +7246,7 @@
       <c r="AA95" s="7"/>
       <c r="AB95" s="7"/>
     </row>
-    <row r="96" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -7281,7 +7281,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="97" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -7344,7 +7344,7 @@
       <c r="AA98" s="5"/>
       <c r="AB98" s="5"/>
     </row>
-    <row r="99" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -7382,7 +7382,7 @@
       <c r="AA99" s="7"/>
       <c r="AB99" s="7"/>
     </row>
-    <row r="100" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="101" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -7440,7 +7440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -7463,7 +7463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -7524,7 +7524,7 @@
       <c r="AA104" s="5"/>
       <c r="AB104" s="5"/>
     </row>
-    <row r="105" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -7562,7 +7562,7 @@
       <c r="AA105" s="3"/>
       <c r="AB105" s="3"/>
     </row>
-    <row r="106" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -7602,7 +7602,7 @@
       <c r="AA106" s="11"/>
       <c r="AB106" s="11"/>
     </row>
-    <row r="107" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -7640,7 +7640,7 @@
       <c r="AA107" s="7"/>
       <c r="AB107" s="7"/>
     </row>
-    <row r="108" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -7669,7 +7669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -7692,7 +7692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -7730,7 +7730,7 @@
       <c r="AA110" s="5"/>
       <c r="AB110" s="5"/>
     </row>
-    <row r="111" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -7768,7 +7768,7 @@
       <c r="AA111" s="7"/>
       <c r="AB111" s="7"/>
     </row>
-    <row r="112" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -7806,7 +7806,7 @@
       <c r="AA112" s="7"/>
       <c r="AB112" s="7"/>
     </row>
-    <row r="113" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -7835,7 +7835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -7861,7 +7861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -7899,7 +7899,7 @@
       <c r="AA115" s="5"/>
       <c r="AB115" s="5"/>
     </row>
-    <row r="116" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -7937,7 +7937,7 @@
       <c r="AA116" s="7"/>
       <c r="AB116" s="7"/>
     </row>
-    <row r="117" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -7975,7 +7975,7 @@
       <c r="AA117" s="7"/>
       <c r="AB117" s="7"/>
     </row>
-    <row r="118" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -8013,7 +8013,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="119" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -8036,7 +8036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -8074,7 +8074,7 @@
       <c r="AA120" s="5"/>
       <c r="AB120" s="5"/>
     </row>
-    <row r="121" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -8109,7 +8109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -8147,7 +8147,7 @@
       <c r="AA122" s="7"/>
       <c r="AB122" s="7"/>
     </row>
-    <row r="123" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -8176,7 +8176,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -8199,7 +8199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -8237,7 +8237,7 @@
       <c r="AA125" s="5"/>
       <c r="AB125" s="5"/>
     </row>
-    <row r="126" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -8269,7 +8269,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -8307,7 +8307,7 @@
       <c r="AA127" s="5"/>
       <c r="AB127" s="5"/>
     </row>
-    <row r="128" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -8345,7 +8345,7 @@
       <c r="AA128" s="5"/>
       <c r="AB128" s="5"/>
     </row>
-    <row r="129" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -8383,7 +8383,7 @@
       <c r="AA129" s="7"/>
       <c r="AB129" s="7"/>
     </row>
-    <row r="130" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -8409,7 +8409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -8438,7 +8438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -8458,7 +8458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -8484,7 +8484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -8507,7 +8507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -8545,7 +8545,7 @@
       <c r="AA135" s="5"/>
       <c r="AB135" s="5"/>
     </row>
-    <row r="136" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -8583,7 +8583,7 @@
       <c r="AA136" s="3"/>
       <c r="AB136" s="3"/>
     </row>
-    <row r="137" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -8623,7 +8623,7 @@
       <c r="AA137" s="11"/>
       <c r="AB137" s="11"/>
     </row>
-    <row r="138" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -8652,7 +8652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -8675,7 +8675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -8713,7 +8713,7 @@
       <c r="AA140" s="7"/>
       <c r="AB140" s="7"/>
     </row>
-    <row r="141" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -8730,7 +8730,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="142" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -8756,7 +8756,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="143" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -8782,7 +8782,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="144" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -8802,7 +8802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -8828,7 +8828,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="146" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -8848,7 +8848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -8868,7 +8868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -8882,7 +8882,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="149" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -8896,7 +8896,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="150" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -8919,7 +8919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -8942,7 +8942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -8980,7 +8980,7 @@
       <c r="AA152" s="7"/>
       <c r="AB152" s="7"/>
     </row>
-    <row r="153" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -9009,7 +9009,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -9047,7 +9047,7 @@
       <c r="AA154" s="5"/>
       <c r="AB154" s="5"/>
     </row>
-    <row r="155" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -9085,7 +9085,7 @@
       <c r="AA155" s="7"/>
       <c r="AB155" s="7"/>
     </row>
-    <row r="156" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -9114,7 +9114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -9152,7 +9152,7 @@
       <c r="AA157" s="5"/>
       <c r="AB157" s="5"/>
     </row>
-    <row r="158" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -9181,7 +9181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="159" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -9219,7 +9219,7 @@
       <c r="AA159" s="5"/>
       <c r="AB159" s="5"/>
     </row>
-    <row r="160" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -9257,7 +9257,7 @@
       <c r="AA160" s="3"/>
       <c r="AB160" s="3"/>
     </row>
-    <row r="161" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -9297,7 +9297,7 @@
       <c r="AA161" s="11"/>
       <c r="AB161" s="11"/>
     </row>
-    <row r="162" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -9326,7 +9326,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -9358,7 +9358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -9398,7 +9398,7 @@
       <c r="AA164" s="7"/>
       <c r="AB164" s="7"/>
     </row>
-    <row r="165" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -9427,7 +9427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -9444,7 +9444,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="167" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -9482,7 +9482,7 @@
       <c r="AA167" s="5"/>
       <c r="AB167" s="5"/>
     </row>
-    <row r="168" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -9514,7 +9514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -9537,7 +9537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -9575,7 +9575,7 @@
       <c r="AA170" s="3"/>
       <c r="AB170" s="3"/>
     </row>
-    <row r="171" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -9615,7 +9615,7 @@
       <c r="AA171" s="11"/>
       <c r="AB171" s="11"/>
     </row>
-    <row r="172" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -9644,7 +9644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -9667,7 +9667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -9693,7 +9693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="175" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -9713,7 +9713,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="176" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -9733,7 +9733,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="177" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -9753,7 +9753,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="178" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -9773,7 +9773,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="179" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -9805,7 +9805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="180" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -9822,7 +9822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="181" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -9851,7 +9851,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -9874,7 +9874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -9912,7 +9912,7 @@
       <c r="AA183" s="5"/>
       <c r="AB183" s="5"/>
     </row>
-    <row r="184" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -9941,7 +9941,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="185" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -9961,7 +9961,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="186" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -9984,7 +9984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -10022,7 +10022,7 @@
       <c r="AA187" s="7"/>
       <c r="AB187" s="7"/>
     </row>
-    <row r="188" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -10051,7 +10051,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -10083,7 +10083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -10106,7 +10106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:28" s="16" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:28" s="16" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -10126,7 +10126,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="192" spans="1:28" s="16" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:28" s="16" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -10146,7 +10146,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="193" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -10166,7 +10166,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="194" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -10186,7 +10186,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="195" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -10209,7 +10209,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="196" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -10247,7 +10247,7 @@
       <c r="AA196" s="5"/>
       <c r="AB196" s="5"/>
     </row>
-    <row r="197" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -10287,7 +10287,7 @@
       <c r="AA197" s="7"/>
       <c r="AB197" s="7"/>
     </row>
-    <row r="198" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -10316,7 +10316,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="199" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -10354,7 +10354,7 @@
       <c r="AA199" s="5"/>
       <c r="AB199" s="5"/>
     </row>
-    <row r="200" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -10377,7 +10377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="201" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -10409,7 +10409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -10432,7 +10432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -10470,7 +10470,7 @@
       <c r="AA203" s="7"/>
       <c r="AB203" s="7"/>
     </row>
-    <row r="204" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -10487,7 +10487,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="205" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -10510,7 +10510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>205</v>
       </c>
@@ -10533,7 +10533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>206</v>
       </c>
@@ -10556,7 +10556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>207</v>
       </c>
@@ -10573,7 +10573,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="209" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>208</v>
       </c>
@@ -10593,7 +10593,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="210" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>209</v>
       </c>
@@ -10616,7 +10616,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="211" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>210</v>
       </c>
@@ -10633,7 +10633,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="212" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>211</v>
       </c>
@@ -10656,7 +10656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>212</v>
       </c>
@@ -10679,7 +10679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>213</v>
       </c>
@@ -10702,7 +10702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>214</v>
       </c>
@@ -10740,7 +10740,7 @@
       <c r="AA215" s="5"/>
       <c r="AB215" s="5"/>
     </row>
-    <row r="216" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>215</v>
       </c>
@@ -10780,7 +10780,7 @@
       <c r="AA216" s="7"/>
       <c r="AB216" s="7"/>
     </row>
-    <row r="217" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>216</v>
       </c>
@@ -10809,7 +10809,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="218" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>217</v>
       </c>
@@ -10838,7 +10838,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>218</v>
       </c>
@@ -10867,7 +10867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="220" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>219</v>
       </c>
@@ -10896,7 +10896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="221" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>220</v>
       </c>
@@ -10934,7 +10934,7 @@
       <c r="AA221" s="5"/>
       <c r="AB221" s="5"/>
     </row>
-    <row r="222" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>221</v>
       </c>
@@ -10966,7 +10966,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="223" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>222</v>
       </c>
@@ -11004,7 +11004,7 @@
       <c r="AA223" s="7"/>
       <c r="AB223" s="7"/>
     </row>
-    <row r="224" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>223</v>
       </c>
@@ -11033,7 +11033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>224</v>
       </c>
@@ -11056,7 +11056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>225</v>
       </c>
@@ -11070,7 +11070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>226</v>
       </c>
@@ -11110,7 +11110,7 @@
       <c r="AA227" s="7"/>
       <c r="AB227" s="7"/>
     </row>
-    <row r="228" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>227</v>
       </c>
@@ -11139,7 +11139,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="229" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>228</v>
       </c>
@@ -11177,7 +11177,7 @@
       <c r="AA229" s="5"/>
       <c r="AB229" s="5"/>
     </row>
-    <row r="230" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>229</v>
       </c>
@@ -11209,7 +11209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>230</v>
       </c>
@@ -11232,7 +11232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>231</v>
       </c>
@@ -11255,7 +11255,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="233" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>232</v>
       </c>
@@ -11287,7 +11287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>233</v>
       </c>
@@ -11310,7 +11310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>234</v>
       </c>
@@ -11348,7 +11348,7 @@
       <c r="AA235" s="3"/>
       <c r="AB235" s="3"/>
     </row>
-    <row r="236" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>235</v>
       </c>
@@ -11388,7 +11388,7 @@
       <c r="AA236" s="11"/>
       <c r="AB236" s="11"/>
     </row>
-    <row r="237" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>236</v>
       </c>
@@ -11426,7 +11426,7 @@
       <c r="AA237" s="7"/>
       <c r="AB237" s="7"/>
     </row>
-    <row r="238" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>237</v>
       </c>
@@ -11455,7 +11455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>238</v>
       </c>
@@ -11478,7 +11478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>239</v>
       </c>
@@ -11516,7 +11516,7 @@
       <c r="AA240" s="5"/>
       <c r="AB240" s="5"/>
     </row>
-    <row r="241" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>240</v>
       </c>
@@ -11554,7 +11554,7 @@
       <c r="AA241" s="7"/>
       <c r="AB241" s="7"/>
     </row>
-    <row r="242" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>241</v>
       </c>
@@ -11583,7 +11583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>242</v>
       </c>
@@ -11606,7 +11606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>243</v>
       </c>
@@ -11644,7 +11644,7 @@
       <c r="AA244" s="5"/>
       <c r="AB244" s="5"/>
     </row>
-    <row r="245" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>244</v>
       </c>
@@ -11682,7 +11682,7 @@
       <c r="AA245" s="7"/>
       <c r="AB245" s="7"/>
     </row>
-    <row r="246" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>245</v>
       </c>
@@ -11705,7 +11705,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="247" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>246</v>
       </c>
@@ -11728,7 +11728,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="248" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>247</v>
       </c>
@@ -11751,7 +11751,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="249" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>248</v>
       </c>
@@ -11774,7 +11774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="250" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>249</v>
       </c>
@@ -11797,7 +11797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="251" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>250</v>
       </c>
@@ -11835,7 +11835,7 @@
       <c r="AA251" s="5"/>
       <c r="AB251" s="5"/>
     </row>
-    <row r="252" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>251</v>
       </c>
@@ -11873,7 +11873,7 @@
       <c r="AA252" s="7"/>
       <c r="AB252" s="7"/>
     </row>
-    <row r="253" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>252</v>
       </c>
@@ -11896,7 +11896,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="254" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>253</v>
       </c>
@@ -11919,7 +11919,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="255" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>254</v>
       </c>
@@ -11942,7 +11942,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>255</v>
       </c>
@@ -11965,7 +11965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="257" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>256</v>
       </c>
@@ -11988,7 +11988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="258" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>257</v>
       </c>
@@ -12026,7 +12026,7 @@
       <c r="AA258" s="5"/>
       <c r="AB258" s="5"/>
     </row>
-    <row r="259" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>258</v>
       </c>
@@ -12062,7 +12062,7 @@
       <c r="AA259" s="7"/>
       <c r="AB259" s="7"/>
     </row>
-    <row r="260" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>259</v>
       </c>
@@ -12091,7 +12091,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="261" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>260</v>
       </c>
@@ -12120,7 +12120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="262" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>261</v>
       </c>
@@ -12149,7 +12149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>262</v>
       </c>
@@ -12172,7 +12172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>263</v>
       </c>
@@ -12201,7 +12201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>264</v>
       </c>
@@ -12224,7 +12224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>265</v>
       </c>
@@ -12262,7 +12262,7 @@
       <c r="AA266" s="5"/>
       <c r="AB266" s="5"/>
     </row>
-    <row r="267" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>266</v>
       </c>
@@ -12291,7 +12291,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="268" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>267</v>
       </c>
@@ -12331,7 +12331,7 @@
       <c r="AA268" s="7"/>
       <c r="AB268" s="7"/>
     </row>
-    <row r="269" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>268</v>
       </c>
@@ -12360,7 +12360,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="270" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>269</v>
       </c>
@@ -12398,7 +12398,7 @@
       <c r="AA270" s="5"/>
       <c r="AB270" s="5"/>
     </row>
-    <row r="271" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>270</v>
       </c>
@@ -12430,7 +12430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>271</v>
       </c>
@@ -12453,7 +12453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>272</v>
       </c>
@@ -12491,7 +12491,7 @@
       <c r="AA273" s="3"/>
       <c r="AB273" s="3"/>
     </row>
-    <row r="274" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>273</v>
       </c>
@@ -12531,7 +12531,7 @@
       <c r="AA274" s="11"/>
       <c r="AB274" s="11"/>
     </row>
-    <row r="275" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>274</v>
       </c>
@@ -12563,7 +12563,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="276" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>275</v>
       </c>
@@ -12601,7 +12601,7 @@
       <c r="AA276" s="7"/>
       <c r="AB276" s="7"/>
     </row>
-    <row r="277" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>276</v>
       </c>
@@ -12630,7 +12630,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="278" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>277</v>
       </c>
@@ -12668,7 +12668,7 @@
       <c r="AA278" s="5"/>
       <c r="AB278" s="5"/>
     </row>
-    <row r="279" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>278</v>
       </c>
@@ -12697,7 +12697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>279</v>
       </c>
@@ -12720,7 +12720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>280</v>
       </c>
@@ -12758,7 +12758,7 @@
       <c r="AA281" s="3"/>
       <c r="AB281" s="3"/>
     </row>
-    <row r="282" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>281</v>
       </c>
@@ -12798,7 +12798,7 @@
       <c r="AA282" s="11"/>
       <c r="AB282" s="11"/>
     </row>
-    <row r="283" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>282</v>
       </c>
@@ -12836,7 +12836,7 @@
       <c r="AA283" s="7"/>
       <c r="AB283" s="7"/>
     </row>
-    <row r="284" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>283</v>
       </c>
@@ -12865,7 +12865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>284</v>
       </c>
@@ -12888,7 +12888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>285</v>
       </c>
@@ -12914,7 +12914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>286</v>
       </c>
@@ -12954,7 +12954,7 @@
       <c r="AA287" s="7"/>
       <c r="AB287" s="7"/>
     </row>
-    <row r="288" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>287</v>
       </c>
@@ -12977,7 +12977,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="289" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>288</v>
       </c>
@@ -13000,7 +13000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="290" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>289</v>
       </c>
@@ -13023,7 +13023,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="291" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>290</v>
       </c>
@@ -13046,7 +13046,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="292" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>291</v>
       </c>
@@ -13069,7 +13069,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="293" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>292</v>
       </c>
@@ -13107,7 +13107,7 @@
       <c r="AA293" s="5"/>
       <c r="AB293" s="5"/>
     </row>
-    <row r="294" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>293</v>
       </c>
@@ -13145,7 +13145,7 @@
       <c r="AA294" s="5"/>
       <c r="AB294" s="5"/>
     </row>
-    <row r="295" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>294</v>
       </c>
@@ -13168,7 +13168,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="296" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>295</v>
       </c>
@@ -13197,7 +13197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="297" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>296</v>
       </c>
@@ -13220,7 +13220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="298" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>297</v>
       </c>
@@ -13249,7 +13249,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="299" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>298</v>
       </c>
@@ -13272,7 +13272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="300" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>299</v>
       </c>
@@ -13295,7 +13295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="301" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>300</v>
       </c>
@@ -13335,7 +13335,7 @@
       <c r="AA301" s="7"/>
       <c r="AB301" s="7"/>
     </row>
-    <row r="302" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>301</v>
       </c>
@@ -13364,7 +13364,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="303" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>302</v>
       </c>
@@ -13402,7 +13402,7 @@
       <c r="AA303" s="5"/>
       <c r="AB303" s="5"/>
     </row>
-    <row r="304" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>303</v>
       </c>
@@ -13431,7 +13431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>304</v>
       </c>
@@ -13454,7 +13454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>305</v>
       </c>
@@ -13483,7 +13483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>306</v>
       </c>
@@ -13506,7 +13506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>307</v>
       </c>
@@ -13544,7 +13544,7 @@
       <c r="AA308" s="3"/>
       <c r="AB308" s="3"/>
     </row>
-    <row r="309" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>308</v>
       </c>
@@ -13584,7 +13584,7 @@
       <c r="AA309" s="11"/>
       <c r="AB309" s="11"/>
     </row>
-    <row r="310" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>309</v>
       </c>
@@ -13622,7 +13622,7 @@
       <c r="AA310" s="7"/>
       <c r="AB310" s="7"/>
     </row>
-    <row r="311" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>310</v>
       </c>
@@ -13651,7 +13651,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="312" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>311</v>
       </c>
@@ -13674,7 +13674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>312</v>
       </c>
@@ -13712,7 +13712,7 @@
       <c r="AA313" s="5"/>
       <c r="AB313" s="5"/>
     </row>
-    <row r="314" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>313</v>
       </c>
@@ -13748,7 +13748,7 @@
       <c r="AA314" s="7"/>
       <c r="AB314" s="7"/>
     </row>
-    <row r="315" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>314</v>
       </c>
@@ -13777,7 +13777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="316" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>315</v>
       </c>
@@ -13806,7 +13806,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="317" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>316</v>
       </c>
@@ -13835,7 +13835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="318" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>317</v>
       </c>
@@ -13864,7 +13864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="319" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>318</v>
       </c>
@@ -13893,7 +13893,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="320" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>319</v>
       </c>
@@ -13922,7 +13922,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="321" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>320</v>
       </c>
@@ -13951,7 +13951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="322" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>321</v>
       </c>
@@ -13980,7 +13980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="323" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>322</v>
       </c>
@@ -14006,7 +14006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="324" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>323</v>
       </c>
@@ -14038,7 +14038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>324</v>
       </c>
@@ -14061,7 +14061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>325</v>
       </c>
@@ -14093,7 +14093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>326</v>
       </c>
@@ -14116,7 +14116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>327</v>
       </c>
@@ -14148,7 +14148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>328</v>
       </c>
@@ -14171,7 +14171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>329</v>
       </c>
@@ -14203,7 +14203,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="331" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>330</v>
       </c>
@@ -14241,7 +14241,7 @@
       <c r="AA331" s="5"/>
       <c r="AB331" s="5"/>
     </row>
-    <row r="332" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>331</v>
       </c>
@@ -14270,7 +14270,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="333" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>332</v>
       </c>
@@ -14310,7 +14310,7 @@
       <c r="AA333" s="7"/>
       <c r="AB333" s="7"/>
     </row>
-    <row r="334" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>333</v>
       </c>
@@ -14339,7 +14339,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="335" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>334</v>
       </c>
@@ -14362,7 +14362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="336" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>335</v>
       </c>
@@ -14400,7 +14400,7 @@
       <c r="AA336" s="5"/>
       <c r="AB336" s="5"/>
     </row>
-    <row r="337" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>336</v>
       </c>
@@ -14438,7 +14438,7 @@
       <c r="AA337" s="3"/>
       <c r="AB337" s="3"/>
     </row>
-    <row r="338" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>337</v>
       </c>
@@ -14478,7 +14478,7 @@
       <c r="AA338" s="11"/>
       <c r="AB338" s="11"/>
     </row>
-    <row r="339" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>338</v>
       </c>
@@ -14516,7 +14516,7 @@
       <c r="AA339" s="7"/>
       <c r="AB339" s="7"/>
     </row>
-    <row r="340" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>339</v>
       </c>
@@ -14545,7 +14545,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="341" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>340</v>
       </c>
@@ -14568,7 +14568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>341</v>
       </c>
@@ -14597,7 +14597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="343" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>342</v>
       </c>
@@ -14611,7 +14611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>343</v>
       </c>
@@ -14649,7 +14649,7 @@
       <c r="AA344" s="7"/>
       <c r="AB344" s="7"/>
     </row>
-    <row r="345" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>344</v>
       </c>
@@ -14678,7 +14678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>345</v>
       </c>
@@ -14701,7 +14701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>346</v>
       </c>
@@ -14724,7 +14724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>347</v>
       </c>
@@ -14747,7 +14747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>348</v>
       </c>
@@ -14785,7 +14785,7 @@
       <c r="AA349" s="5"/>
       <c r="AB349" s="5"/>
     </row>
-    <row r="350" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>349</v>
       </c>
@@ -14825,7 +14825,7 @@
       <c r="AA350" s="7"/>
       <c r="AB350" s="7"/>
     </row>
-    <row r="351" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>350</v>
       </c>
@@ -14857,7 +14857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>351</v>
       </c>
@@ -14880,7 +14880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>352</v>
       </c>
@@ -14918,7 +14918,7 @@
       <c r="AA353" s="5"/>
       <c r="AB353" s="5"/>
     </row>
-    <row r="354" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>353</v>
       </c>
@@ -14956,7 +14956,7 @@
       <c r="AA354" s="7"/>
       <c r="AB354" s="7"/>
     </row>
-    <row r="355" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <v>354</v>
       </c>
@@ -14985,7 +14985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="356" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <v>355</v>
       </c>
@@ -15014,7 +15014,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="357" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <v>356</v>
       </c>
@@ -15043,7 +15043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
         <v>357</v>
       </c>
@@ -15066,7 +15066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
         <v>358</v>
       </c>
@@ -15104,7 +15104,7 @@
       <c r="AA359" s="5"/>
       <c r="AB359" s="5"/>
     </row>
-    <row r="360" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>359</v>
       </c>
@@ -15142,7 +15142,7 @@
       <c r="AA360" s="3"/>
       <c r="AB360" s="3"/>
     </row>
-    <row r="361" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <v>360</v>
       </c>
@@ -15182,7 +15182,7 @@
       <c r="AA361" s="11"/>
       <c r="AB361" s="11"/>
     </row>
-    <row r="362" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <v>361</v>
       </c>
@@ -15220,7 +15220,7 @@
       <c r="AA362" s="7"/>
       <c r="AB362" s="7"/>
     </row>
-    <row r="363" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <v>362</v>
       </c>
@@ -15249,7 +15249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>363</v>
       </c>
@@ -15272,7 +15272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <v>364</v>
       </c>
@@ -15298,7 +15298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="366" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>365</v>
       </c>
@@ -15336,7 +15336,7 @@
       <c r="AA366" s="5"/>
       <c r="AB366" s="5"/>
     </row>
-    <row r="367" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
         <v>366</v>
       </c>
@@ -15368,7 +15368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="1">
         <v>367</v>
       </c>
@@ -15391,7 +15391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A369" s="1">
         <v>368</v>
       </c>
@@ -15429,7 +15429,7 @@
       <c r="AA369" s="3"/>
       <c r="AB369" s="3"/>
     </row>
-    <row r="370" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
         <v>369</v>
       </c>
@@ -15469,7 +15469,7 @@
       <c r="AA370" s="11"/>
       <c r="AB370" s="11"/>
     </row>
-    <row r="371" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A371" s="1">
         <v>370</v>
       </c>
@@ -15505,7 +15505,7 @@
       <c r="AA371" s="7"/>
       <c r="AB371" s="7"/>
     </row>
-    <row r="372" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
         <v>371</v>
       </c>
@@ -15534,7 +15534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="373" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
         <v>372</v>
       </c>
@@ -15563,7 +15563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A374" s="1">
         <v>373</v>
       </c>
@@ -15586,7 +15586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A375" s="1">
         <v>374</v>
       </c>
@@ -15624,7 +15624,7 @@
       <c r="AA375" s="5"/>
       <c r="AB375" s="5"/>
     </row>
-    <row r="376" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A376" s="1">
         <v>375</v>
       </c>
@@ -15662,7 +15662,7 @@
       <c r="AA376" s="3"/>
       <c r="AB376" s="3"/>
     </row>
-    <row r="377" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A377" s="1">
         <v>376</v>
       </c>
@@ -15702,7 +15702,7 @@
       <c r="AA377" s="11"/>
       <c r="AB377" s="11"/>
     </row>
-    <row r="378" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A378" s="1">
         <v>377</v>
       </c>
@@ -15740,7 +15740,7 @@
       <c r="AA378" s="7"/>
       <c r="AB378" s="7"/>
     </row>
-    <row r="379" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A379" s="1">
         <v>378</v>
       </c>
@@ -15769,7 +15769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A380" s="1">
         <v>379</v>
       </c>
@@ -15792,7 +15792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A381" s="1">
         <v>380</v>
       </c>
@@ -15830,7 +15830,7 @@
       <c r="AA381" s="5"/>
       <c r="AB381" s="5"/>
     </row>
-    <row r="382" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A382" s="1">
         <v>381</v>
       </c>
@@ -15868,7 +15868,7 @@
       <c r="AA382" s="7"/>
       <c r="AB382" s="7"/>
     </row>
-    <row r="383" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A383" s="1">
         <v>382</v>
       </c>
@@ -15897,7 +15897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A384" s="1">
         <v>383</v>
       </c>
@@ -15920,7 +15920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="385" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A385" s="1">
         <v>384</v>
       </c>
@@ -15958,7 +15958,7 @@
       <c r="AA385" s="5"/>
       <c r="AB385" s="5"/>
     </row>
-    <row r="386" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A386" s="1">
         <v>385</v>
       </c>
@@ -15990,7 +15990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="387" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
         <v>386</v>
       </c>
@@ -16013,7 +16013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="388" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A388" s="1">
         <v>387</v>
       </c>
@@ -16042,7 +16042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="389" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A389" s="1">
         <v>388</v>
       </c>
@@ -16065,7 +16065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="390" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A390" s="1">
         <v>389</v>
       </c>
@@ -16094,7 +16094,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="391" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A391" s="1">
         <v>390</v>
       </c>
@@ -16117,7 +16117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="392" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
         <v>391</v>
       </c>
@@ -16149,7 +16149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="393" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A393" s="1">
         <v>392</v>
       </c>
@@ -16172,7 +16172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="394" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A394" s="1">
         <v>393</v>
       </c>
@@ -16195,7 +16195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="395" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
         <v>394</v>
       </c>
@@ -16218,7 +16218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="396" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
         <v>395</v>
       </c>
@@ -16247,7 +16247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="397" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
         <v>396</v>
       </c>
@@ -16270,7 +16270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
         <v>397</v>
       </c>
@@ -16299,7 +16299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="399" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A399" s="1">
         <v>398</v>
       </c>
@@ -16322,7 +16322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="400" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="1">
         <v>399</v>
       </c>
@@ -16360,7 +16360,7 @@
       <c r="AA400" s="3"/>
       <c r="AB400" s="3"/>
     </row>
-    <row r="401" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A401" s="1">
         <v>400</v>
       </c>
@@ -16398,7 +16398,7 @@
       <c r="AA401" s="11"/>
       <c r="AB401" s="11"/>
     </row>
-    <row r="402" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
         <v>401</v>
       </c>
@@ -16421,7 +16421,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="403" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A403" s="1">
         <v>402</v>
       </c>
@@ -16444,7 +16444,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="404" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
         <v>403</v>
       </c>
@@ -16467,7 +16467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="405" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
         <v>404</v>
       </c>
@@ -16490,7 +16490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="406" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
         <v>405</v>
       </c>
@@ -16516,7 +16516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="407" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
         <v>406</v>
       </c>
@@ -16554,7 +16554,7 @@
       <c r="AA407" s="3"/>
       <c r="AB407" s="3"/>
     </row>
-    <row r="408" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A408" s="1">
         <v>407</v>
       </c>
@@ -16571,7 +16571,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="409" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A409" s="1">
         <v>408</v>
       </c>
@@ -16609,7 +16609,7 @@
       <c r="AA409" s="3"/>
       <c r="AB409" s="3"/>
     </row>
-    <row r="410" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A410" s="1">
         <v>409</v>
       </c>
@@ -16649,7 +16649,7 @@
       <c r="AA410" s="11"/>
       <c r="AB410" s="11"/>
     </row>
-    <row r="411" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A411" s="1">
         <v>410</v>
       </c>
@@ -16687,7 +16687,7 @@
       <c r="AA411" s="7"/>
       <c r="AB411" s="7"/>
     </row>
-    <row r="412" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A412" s="1">
         <v>411</v>
       </c>
@@ -16716,7 +16716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="413" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A413" s="1">
         <v>412</v>
       </c>
@@ -16745,7 +16745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="414" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A414" s="1">
         <v>413</v>
       </c>
@@ -16774,7 +16774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="415" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A415" s="1">
         <v>414</v>
       </c>
@@ -16803,7 +16803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="416" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A416" s="1">
         <v>415</v>
       </c>
@@ -16832,7 +16832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="417" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A417" s="1">
         <v>416</v>
       </c>
@@ -16861,7 +16861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="418" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
         <v>417</v>
       </c>
@@ -16899,7 +16899,7 @@
       <c r="AA418" s="5"/>
       <c r="AB418" s="5"/>
     </row>
-    <row r="419" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A419" s="1">
         <v>418</v>
       </c>
@@ -16937,7 +16937,7 @@
       <c r="AA419" s="7"/>
       <c r="AB419" s="7"/>
     </row>
-    <row r="420" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A420" s="1">
         <v>419</v>
       </c>
@@ -16960,7 +16960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="421" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
         <v>420</v>
       </c>
@@ -16998,7 +16998,7 @@
       <c r="AA421" s="5"/>
       <c r="AB421" s="5"/>
     </row>
-    <row r="422" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
         <v>421</v>
       </c>
@@ -17015,7 +17015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="423" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A423" s="1">
         <v>422</v>
       </c>
@@ -17053,7 +17053,7 @@
       <c r="AA423" s="3"/>
       <c r="AB423" s="3"/>
     </row>
-    <row r="424" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:28" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A424" s="1">
         <v>423</v>
       </c>
@@ -17102,54 +17102,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="108" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.08984375" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.453125" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.453125" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.90625" style="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="123.453125" style="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.81640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.26953125" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.26953125" style="30" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.7265625" style="30" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.36328125" style="30" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.90625" style="30" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.1796875" style="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.1796875" style="30" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.7265625" style="30" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.81640625" style="30"/>
+    <col min="1" max="1" width="8.21875" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50" style="30" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="30" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="30.88671875" style="30" customWidth="1"/>
+    <col min="9" max="9" width="8.77734375" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.21875" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.21875" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.77734375" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" style="30" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="18.21875" style="30" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="4.21875" style="30" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="22.77734375" style="30" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.77734375" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="43" customFormat="1" ht="11" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:17" s="43" customFormat="1" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="54" t="s">
         <v>1155</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-    </row>
-    <row r="2" spans="1:17" s="43" customFormat="1" ht="11" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+    </row>
+    <row r="2" spans="1:17" s="43" customFormat="1" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="46" t="s">
         <v>1150</v>
       </c>
@@ -17202,7 +17203,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="135.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>1133</v>
       </c>
@@ -17237,7 +17238,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="110.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="30" t="s">
         <v>1133</v>
       </c>
@@ -17267,28 +17268,28 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="31" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="57" t="s">
+    <row r="5" spans="1:17" s="31" customFormat="1" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="59" t="s">
         <v>1151</v>
       </c>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="60"/>
-    </row>
-    <row r="6" spans="1:17" s="31" customFormat="1" ht="11" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="62"/>
+    </row>
+    <row r="6" spans="1:17" s="31" customFormat="1" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>1150</v>
       </c>
@@ -17301,14 +17302,14 @@
       <c r="D6" s="34" t="s">
         <v>1147</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="63" t="s">
         <v>1146</v>
       </c>
-      <c r="F6" s="62"/>
-      <c r="G6" s="63" t="s">
+      <c r="F6" s="64"/>
+      <c r="G6" s="65" t="s">
         <v>1145</v>
       </c>
-      <c r="H6" s="63"/>
+      <c r="H6" s="65"/>
       <c r="I6" s="33" t="s">
         <v>1144</v>
       </c>
@@ -17337,21 +17338,21 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="1" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1133</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1168</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="57" t="s">
         <v>1130</v>
       </c>
-      <c r="F7" s="54"/>
-      <c r="G7" s="55" t="s">
+      <c r="F7" s="57"/>
+      <c r="G7" s="58" t="s">
         <v>1131</v>
       </c>
-      <c r="H7" s="55"/>
+      <c r="H7" s="58"/>
       <c r="K7" s="51" t="s">
         <v>232</v>
       </c>
@@ -17365,21 +17366,21 @@
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="1" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1133</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>1135</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="E8" s="57" t="s">
         <v>1130</v>
       </c>
-      <c r="F8" s="54"/>
-      <c r="G8" s="55" t="s">
+      <c r="F8" s="57"/>
+      <c r="G8" s="58" t="s">
         <v>1131</v>
       </c>
-      <c r="H8" s="55"/>
+      <c r="H8" s="58"/>
       <c r="K8" s="51" t="s">
         <v>224</v>
       </c>
@@ -17393,21 +17394,21 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="1" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="1" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1133</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>1134</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="E9" s="57" t="s">
         <v>1131</v>
       </c>
-      <c r="F9" s="54"/>
-      <c r="G9" s="55" t="s">
+      <c r="F9" s="57"/>
+      <c r="G9" s="58" t="s">
         <v>1130</v>
       </c>
-      <c r="H9" s="55"/>
+      <c r="H9" s="58"/>
       <c r="K9" s="51" t="s">
         <v>196</v>
       </c>
@@ -17421,21 +17422,21 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="1" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="1" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1133</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="E10" s="57" t="s">
         <v>1131</v>
       </c>
-      <c r="F10" s="54"/>
-      <c r="G10" s="55" t="s">
+      <c r="F10" s="57"/>
+      <c r="G10" s="58" t="s">
         <v>1130</v>
       </c>
-      <c r="H10" s="55"/>
+      <c r="H10" s="58"/>
       <c r="K10" s="51" t="s">
         <v>193</v>
       </c>
@@ -17449,21 +17450,21 @@
         <v>194</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
         <v>1156</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>1160</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="55" t="s">
         <v>1159</v>
       </c>
-      <c r="F11" s="64"/>
-      <c r="G11" s="65" t="s">
+      <c r="F11" s="55"/>
+      <c r="G11" s="56" t="s">
         <v>1158</v>
       </c>
-      <c r="H11" s="65"/>
+      <c r="H11" s="56"/>
       <c r="K11" s="2" t="s">
         <v>167</v>
       </c>
@@ -17478,21 +17479,20 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="13">
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A5:Q5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A5:Q5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <conditionalFormatting sqref="R1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>